<commit_message>
Added model accuracy plots, learning curves, and extracted features
</commit_message>
<xml_diff>
--- a/results/results.xlsx
+++ b/results/results.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sue_lynne/Documents/Projects/2021-22/results/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{870D50A0-0481-EB42-BB9D-E5EEAAEA30C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE4A62F4-ABA2-3944-91A7-37B1B906187E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="800" yWindow="700" windowWidth="27640" windowHeight="16440" xr2:uid="{0BC0DAEB-F4A9-1941-8A5E-FCBBDF41CE1C}"/>
+    <workbookView xWindow="800" yWindow="700" windowWidth="27640" windowHeight="16440" activeTab="1" xr2:uid="{0BC0DAEB-F4A9-1941-8A5E-FCBBDF41CE1C}"/>
   </bookViews>
   <sheets>
     <sheet name="A" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="114">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="113">
   <si>
     <t>Model</t>
   </si>
@@ -235,33 +235,6 @@
     <t>Test Set F1 Score: 0.2633</t>
   </si>
   <si>
-    <t>Training Set Accuracy Score: 0.7605</t>
-  </si>
-  <si>
-    <t>Validation Set Accuracy Score: 0.6704</t>
-  </si>
-  <si>
-    <t>Validation Set Precision Score: 0.6704</t>
-  </si>
-  <si>
-    <t>Validation Set Recall Score: 0.6704</t>
-  </si>
-  <si>
-    <t>Validation Set F1 Score: 0.6704</t>
-  </si>
-  <si>
-    <t>Test Set Accuracy Score: 0.6700</t>
-  </si>
-  <si>
-    <t>Test Set Precision Score: 0.6700</t>
-  </si>
-  <si>
-    <t>Test Set Recall Score: 0.6700</t>
-  </si>
-  <si>
-    <t>Test Set F1 Score: 0.6700</t>
-  </si>
-  <si>
     <t>SVC(C=1, class_weight='balanced', gamma=1e-9, random_state=0)</t>
   </si>
   <si>
@@ -377,6 +350,30 @@
   </si>
   <si>
     <t>Deep learning models</t>
+  </si>
+  <si>
+    <t>Training Set Accuracy Score: 0.7070</t>
+  </si>
+  <si>
+    <t>Validation Set Accuracy Score: 0.6667</t>
+  </si>
+  <si>
+    <t>Validation Set Precision Score: 0.6667</t>
+  </si>
+  <si>
+    <t>Validation Set Recall Score: 0.6667</t>
+  </si>
+  <si>
+    <t>Test Set Accuracy Score: 0.6333</t>
+  </si>
+  <si>
+    <t>Test Set Precision Score: 0.6333</t>
+  </si>
+  <si>
+    <t>Test Set Recall Score: 0.6333</t>
+  </si>
+  <si>
+    <t>Test Set F1 Score: 0.6333</t>
   </si>
 </sst>
 </file>
@@ -910,8 +907,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D4AE902C-3946-BC42-A752-52CB35AEE6BD}">
   <dimension ref="A1:E27"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="102" workbookViewId="0">
-      <selection activeCell="A30" sqref="A30"/>
+    <sheetView zoomScale="88" workbookViewId="0">
+      <selection activeCell="E24" sqref="E24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -942,7 +939,7 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="16" t="s">
-        <v>112</v>
+        <v>103</v>
       </c>
       <c r="B2" s="17"/>
       <c r="C2" s="17"/>
@@ -957,10 +954,10 @@
         <v>5</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>85</v>
+        <v>76</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>89</v>
+        <v>80</v>
       </c>
       <c r="E3" s="4" t="s">
         <v>11</v>
@@ -969,13 +966,13 @@
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" s="2"/>
       <c r="B4" s="3" t="s">
-        <v>84</v>
+        <v>75</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>86</v>
+        <v>77</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>90</v>
+        <v>81</v>
       </c>
       <c r="E4" s="4"/>
     </row>
@@ -983,10 +980,10 @@
       <c r="A5" s="2"/>
       <c r="B5" s="3"/>
       <c r="C5" s="3" t="s">
-        <v>87</v>
+        <v>78</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>91</v>
+        <v>82</v>
       </c>
       <c r="E5" s="4"/>
     </row>
@@ -994,10 +991,10 @@
       <c r="A6" s="2"/>
       <c r="B6" s="3"/>
       <c r="C6" s="3" t="s">
-        <v>88</v>
+        <v>79</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>92</v>
+        <v>83</v>
       </c>
       <c r="E6" s="4"/>
     </row>
@@ -1009,25 +1006,25 @@
         <v>5</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>77</v>
+        <v>68</v>
       </c>
       <c r="D7" s="6" t="s">
-        <v>80</v>
+        <v>71</v>
       </c>
       <c r="E7" s="7" t="s">
-        <v>76</v>
+        <v>67</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" s="5"/>
       <c r="B8" s="6" t="s">
-        <v>75</v>
+        <v>66</v>
       </c>
       <c r="C8" s="6" t="s">
         <v>16</v>
       </c>
       <c r="D8" s="6" t="s">
-        <v>81</v>
+        <v>72</v>
       </c>
       <c r="E8" s="7"/>
     </row>
@@ -1035,10 +1032,10 @@
       <c r="A9" s="5"/>
       <c r="B9" s="6"/>
       <c r="C9" s="6" t="s">
-        <v>78</v>
+        <v>69</v>
       </c>
       <c r="D9" s="6" t="s">
-        <v>82</v>
+        <v>73</v>
       </c>
       <c r="E9" s="7"/>
     </row>
@@ -1046,16 +1043,16 @@
       <c r="A10" s="8"/>
       <c r="B10" s="9"/>
       <c r="C10" s="9" t="s">
-        <v>79</v>
+        <v>70</v>
       </c>
       <c r="D10" s="9" t="s">
-        <v>83</v>
+        <v>74</v>
       </c>
       <c r="E10" s="10"/>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" s="16" t="s">
-        <v>113</v>
+        <v>104</v>
       </c>
       <c r="B11" s="17"/>
       <c r="C11" s="17"/>
@@ -1263,8 +1260,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DF6B9EBB-1EE7-5045-8496-5244C6CF24D7}">
   <dimension ref="A1:J27"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B29" sqref="B29"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B31" sqref="B31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1296,7 +1293,7 @@
     </row>
     <row r="2" spans="1:10" ht="19" x14ac:dyDescent="0.25">
       <c r="A2" s="16" t="s">
-        <v>112</v>
+        <v>103</v>
       </c>
       <c r="B2" s="17"/>
       <c r="C2" s="17"/>
@@ -1312,26 +1309,26 @@
         <v>5</v>
       </c>
       <c r="C3" s="22" t="s">
-        <v>104</v>
+        <v>95</v>
       </c>
       <c r="D3" s="22" t="s">
-        <v>108</v>
+        <v>99</v>
       </c>
       <c r="E3" s="23" t="s">
-        <v>103</v>
+        <v>94</v>
       </c>
       <c r="J3" s="1"/>
     </row>
     <row r="4" spans="1:10" ht="19" x14ac:dyDescent="0.25">
       <c r="A4" s="21"/>
       <c r="B4" s="22" t="s">
-        <v>84</v>
+        <v>75</v>
       </c>
       <c r="C4" s="22" t="s">
-        <v>105</v>
+        <v>96</v>
       </c>
       <c r="D4" s="22" t="s">
-        <v>109</v>
+        <v>100</v>
       </c>
       <c r="E4" s="23"/>
       <c r="J4" s="1"/>
@@ -1340,10 +1337,10 @@
       <c r="A5" s="21"/>
       <c r="B5" s="22"/>
       <c r="C5" s="22" t="s">
-        <v>106</v>
+        <v>97</v>
       </c>
       <c r="D5" s="22" t="s">
-        <v>110</v>
+        <v>101</v>
       </c>
       <c r="E5" s="23"/>
       <c r="J5" s="1"/>
@@ -1352,10 +1349,10 @@
       <c r="A6" s="21"/>
       <c r="B6" s="22"/>
       <c r="C6" s="22" t="s">
-        <v>107</v>
+        <v>98</v>
       </c>
       <c r="D6" s="22" t="s">
-        <v>111</v>
+        <v>102</v>
       </c>
       <c r="E6" s="23"/>
       <c r="J6" s="1"/>
@@ -1368,26 +1365,26 @@
         <v>5</v>
       </c>
       <c r="C7" s="22" t="s">
-        <v>95</v>
+        <v>86</v>
       </c>
       <c r="D7" s="22" t="s">
-        <v>99</v>
+        <v>90</v>
       </c>
       <c r="E7" s="23" t="s">
-        <v>94</v>
+        <v>85</v>
       </c>
       <c r="J7" s="1"/>
     </row>
     <row r="8" spans="1:10" ht="19" x14ac:dyDescent="0.25">
       <c r="A8" s="21"/>
       <c r="B8" s="22" t="s">
-        <v>93</v>
+        <v>84</v>
       </c>
       <c r="C8" s="22" t="s">
-        <v>96</v>
+        <v>87</v>
       </c>
       <c r="D8" s="22" t="s">
-        <v>100</v>
+        <v>91</v>
       </c>
       <c r="E8" s="23"/>
       <c r="J8" s="1"/>
@@ -1396,10 +1393,10 @@
       <c r="A9" s="21"/>
       <c r="B9" s="22"/>
       <c r="C9" s="22" t="s">
-        <v>97</v>
+        <v>88</v>
       </c>
       <c r="D9" s="22" t="s">
-        <v>101</v>
+        <v>92</v>
       </c>
       <c r="E9" s="23"/>
       <c r="J9" s="1"/>
@@ -1408,16 +1405,16 @@
       <c r="A10" s="24"/>
       <c r="B10" s="25"/>
       <c r="C10" s="25" t="s">
-        <v>98</v>
+        <v>89</v>
       </c>
       <c r="D10" s="25" t="s">
-        <v>102</v>
+        <v>93</v>
       </c>
       <c r="E10" s="26"/>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A11" s="16" t="s">
-        <v>113</v>
+        <v>104</v>
       </c>
       <c r="B11" s="17"/>
       <c r="C11" s="17"/>
@@ -1478,23 +1475,23 @@
       </c>
       <c r="B16" s="3"/>
       <c r="C16" s="3" t="s">
-        <v>67</v>
+        <v>106</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>71</v>
+        <v>109</v>
       </c>
       <c r="E16" s="4" t="s">
-        <v>66</v>
+        <v>105</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17" s="2"/>
       <c r="B17" s="3"/>
       <c r="C17" s="3" t="s">
-        <v>68</v>
+        <v>107</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>72</v>
+        <v>110</v>
       </c>
       <c r="E17" s="4"/>
     </row>
@@ -1502,10 +1499,10 @@
       <c r="A18" s="2"/>
       <c r="B18" s="3"/>
       <c r="C18" s="3" t="s">
-        <v>69</v>
+        <v>108</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>73</v>
+        <v>111</v>
       </c>
       <c r="E18" s="4"/>
     </row>
@@ -1516,7 +1513,7 @@
         <v>70</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>74</v>
+        <v>112</v>
       </c>
       <c r="E19" s="4"/>
     </row>

</xml_diff>